<commit_message>
WIP Add missing parameter entries in xlsx file and AD_IO
Also added the bundled 2D array for each blade and node for BNFam and BNAddMa
</commit_message>
<xml_diff>
--- a/modules/aerodyn/src/OutListParameters.xlsx
+++ b/modules/aerodyn/src/OutListParameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dusti\Documents\prog\PRIMED\FASTInterface Projects\openfastDS\modules\aerodyn\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5A4012-8AC6-4853-9696-91435CD4168C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA5540C-768F-4382-8728-B683E40B49B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="2360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4069" uniqueCount="2442">
   <si>
     <t>Category</t>
   </si>
@@ -7109,6 +7109,252 @@
   </si>
   <si>
     <t>Added mass force at Blade 3, Node 9</t>
+  </si>
+  <si>
+    <t>B1N1Cpmin</t>
+  </si>
+  <si>
+    <t>B1N2Cpmin</t>
+  </si>
+  <si>
+    <t>B1N3Cpmin</t>
+  </si>
+  <si>
+    <t>B1N4Cpmin</t>
+  </si>
+  <si>
+    <t>B1N5Cpmin</t>
+  </si>
+  <si>
+    <t>B1N6Cpmin</t>
+  </si>
+  <si>
+    <t>B1N7Cpmin</t>
+  </si>
+  <si>
+    <t>B1N8Cpmin</t>
+  </si>
+  <si>
+    <t>B1N9Cpmin</t>
+  </si>
+  <si>
+    <t>B2N1Cpmin</t>
+  </si>
+  <si>
+    <t>B2N2Cpmin</t>
+  </si>
+  <si>
+    <t>B2N3Cpmin</t>
+  </si>
+  <si>
+    <t>B2N4Cpmin</t>
+  </si>
+  <si>
+    <t>B2N5Cpmin</t>
+  </si>
+  <si>
+    <t>B2N6Cpmin</t>
+  </si>
+  <si>
+    <t>B2N7Cpmin</t>
+  </si>
+  <si>
+    <t>B2N8Cpmin</t>
+  </si>
+  <si>
+    <t>B2N9Cpmin</t>
+  </si>
+  <si>
+    <t>B3N1Cpmin</t>
+  </si>
+  <si>
+    <t>B3N2Cpmin</t>
+  </si>
+  <si>
+    <t>B3N3Cpmin</t>
+  </si>
+  <si>
+    <t>B3N4Cpmin</t>
+  </si>
+  <si>
+    <t>B3N5Cpmin</t>
+  </si>
+  <si>
+    <t>B3N6Cpmin</t>
+  </si>
+  <si>
+    <t>B3N7Cpmin</t>
+  </si>
+  <si>
+    <t>B3N8Cpmin</t>
+  </si>
+  <si>
+    <t>B3N9Cpmin</t>
+  </si>
+  <si>
+    <t>B1N1SigCr</t>
+  </si>
+  <si>
+    <t>B1N2SigCr</t>
+  </si>
+  <si>
+    <t>B1N3SigCr</t>
+  </si>
+  <si>
+    <t>B1N4SigCr</t>
+  </si>
+  <si>
+    <t>B1N5SigCr</t>
+  </si>
+  <si>
+    <t>B1N6SigCr</t>
+  </si>
+  <si>
+    <t>B1N7SigCr</t>
+  </si>
+  <si>
+    <t>B1N8SigCr</t>
+  </si>
+  <si>
+    <t>B1N9SigCr</t>
+  </si>
+  <si>
+    <t>B2N1SigCr</t>
+  </si>
+  <si>
+    <t>B2N2SigCr</t>
+  </si>
+  <si>
+    <t>B2N3SigCr</t>
+  </si>
+  <si>
+    <t>B2N4SigCr</t>
+  </si>
+  <si>
+    <t>B2N5SigCr</t>
+  </si>
+  <si>
+    <t>B2N6SigCr</t>
+  </si>
+  <si>
+    <t>B2N7SigCr</t>
+  </si>
+  <si>
+    <t>B2N8SigCr</t>
+  </si>
+  <si>
+    <t>B2N9SigCr</t>
+  </si>
+  <si>
+    <t>B3N1SigCr</t>
+  </si>
+  <si>
+    <t>B3N2SigCr</t>
+  </si>
+  <si>
+    <t>B3N3SigCr</t>
+  </si>
+  <si>
+    <t>B3N4SigCr</t>
+  </si>
+  <si>
+    <t>B3N5SigCr</t>
+  </si>
+  <si>
+    <t>B3N6SigCr</t>
+  </si>
+  <si>
+    <t>B3N7SigCr</t>
+  </si>
+  <si>
+    <t>B3N8SigCr</t>
+  </si>
+  <si>
+    <t>B3N9SigCr</t>
+  </si>
+  <si>
+    <t>B1N1SgCav</t>
+  </si>
+  <si>
+    <t>B1N2SgCav</t>
+  </si>
+  <si>
+    <t>B1N3SgCav</t>
+  </si>
+  <si>
+    <t>B1N4SgCav</t>
+  </si>
+  <si>
+    <t>B1N5SgCav</t>
+  </si>
+  <si>
+    <t>B1N6SgCav</t>
+  </si>
+  <si>
+    <t>B1N7SgCav</t>
+  </si>
+  <si>
+    <t>B1N8SgCav</t>
+  </si>
+  <si>
+    <t>B1N9SgCav</t>
+  </si>
+  <si>
+    <t>B2N1SgCav</t>
+  </si>
+  <si>
+    <t>B2N2SgCav</t>
+  </si>
+  <si>
+    <t>B2N3SgCav</t>
+  </si>
+  <si>
+    <t>B2N4SgCav</t>
+  </si>
+  <si>
+    <t>B2N5SgCav</t>
+  </si>
+  <si>
+    <t>B2N6SgCav</t>
+  </si>
+  <si>
+    <t>B2N7SgCav</t>
+  </si>
+  <si>
+    <t>B2N8SgCav</t>
+  </si>
+  <si>
+    <t>B2N9SgCav</t>
+  </si>
+  <si>
+    <t>B3N1SgCav</t>
+  </si>
+  <si>
+    <t>B3N2SgCav</t>
+  </si>
+  <si>
+    <t>B3N3SgCav</t>
+  </si>
+  <si>
+    <t>B3N4SgCav</t>
+  </si>
+  <si>
+    <t>B3N5SgCav</t>
+  </si>
+  <si>
+    <t>B3N6SgCav</t>
+  </si>
+  <si>
+    <t>B3N7SgCav</t>
+  </si>
+  <si>
+    <t>B3N8SgCav</t>
+  </si>
+  <si>
+    <t>B3N9SgCav</t>
+  </si>
+  <si>
+    <t>TODO add note</t>
   </si>
 </sst>
 </file>
@@ -7605,7 +7851,7 @@
       </c>
       <c r="D8">
         <f>COUNTA(AeroDyn!B:B)-1</f>
-        <v>1157</v>
+        <v>1238</v>
       </c>
       <c r="E8" t="s">
         <v>45</v>
@@ -7698,10 +7944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G1161"/>
+  <dimension ref="A1:G1242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1092" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1105" sqref="D1105"/>
+    <sheetView tabSelected="1" topLeftCell="A1140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1159" sqref="E1159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20778,10 +21024,10 @@
     </row>
     <row r="1090" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1090" s="11" t="s">
-        <v>2252</v>
+        <v>2360</v>
       </c>
       <c r="D1090" s="8" t="s">
-        <v>2306</v>
+        <v>2441</v>
       </c>
       <c r="F1090" t="s">
         <v>3</v>
@@ -20789,10 +21035,10 @@
     </row>
     <row r="1091" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1091" s="11" t="s">
-        <v>2253</v>
+        <v>2361</v>
       </c>
       <c r="D1091" s="8" t="s">
-        <v>2307</v>
+        <v>2441</v>
       </c>
       <c r="F1091" t="s">
         <v>3</v>
@@ -20800,10 +21046,10 @@
     </row>
     <row r="1092" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1092" s="11" t="s">
-        <v>2254</v>
+        <v>2362</v>
       </c>
       <c r="D1092" s="8" t="s">
-        <v>2308</v>
+        <v>2441</v>
       </c>
       <c r="F1092" t="s">
         <v>3</v>
@@ -20811,10 +21057,10 @@
     </row>
     <row r="1093" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1093" s="11" t="s">
-        <v>2255</v>
+        <v>2363</v>
       </c>
       <c r="D1093" s="8" t="s">
-        <v>2309</v>
+        <v>2441</v>
       </c>
       <c r="F1093" t="s">
         <v>3</v>
@@ -20822,10 +21068,10 @@
     </row>
     <row r="1094" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1094" s="11" t="s">
-        <v>2256</v>
+        <v>2364</v>
       </c>
       <c r="D1094" s="8" t="s">
-        <v>2310</v>
+        <v>2441</v>
       </c>
       <c r="F1094" t="s">
         <v>3</v>
@@ -20833,10 +21079,10 @@
     </row>
     <row r="1095" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1095" s="11" t="s">
-        <v>2257</v>
+        <v>2365</v>
       </c>
       <c r="D1095" s="8" t="s">
-        <v>2311</v>
+        <v>2441</v>
       </c>
       <c r="F1095" t="s">
         <v>3</v>
@@ -20844,10 +21090,10 @@
     </row>
     <row r="1096" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1096" s="11" t="s">
-        <v>2258</v>
+        <v>2366</v>
       </c>
       <c r="D1096" s="8" t="s">
-        <v>2312</v>
+        <v>2441</v>
       </c>
       <c r="F1096" t="s">
         <v>3</v>
@@ -20855,10 +21101,10 @@
     </row>
     <row r="1097" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1097" s="11" t="s">
-        <v>2259</v>
+        <v>2367</v>
       </c>
       <c r="D1097" s="8" t="s">
-        <v>2313</v>
+        <v>2441</v>
       </c>
       <c r="F1097" t="s">
         <v>3</v>
@@ -20866,10 +21112,10 @@
     </row>
     <row r="1098" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1098" s="11" t="s">
-        <v>2260</v>
+        <v>2368</v>
       </c>
       <c r="D1098" s="8" t="s">
-        <v>2314</v>
+        <v>2441</v>
       </c>
       <c r="F1098" t="s">
         <v>3</v>
@@ -20877,10 +21123,10 @@
     </row>
     <row r="1099" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1099" s="11" t="s">
-        <v>2261</v>
+        <v>2369</v>
       </c>
       <c r="D1099" s="8" t="s">
-        <v>2315</v>
+        <v>2441</v>
       </c>
       <c r="F1099" t="s">
         <v>3</v>
@@ -20888,10 +21134,10 @@
     </row>
     <row r="1100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1100" s="11" t="s">
-        <v>2262</v>
+        <v>2370</v>
       </c>
       <c r="D1100" s="8" t="s">
-        <v>2316</v>
+        <v>2441</v>
       </c>
       <c r="F1100" t="s">
         <v>3</v>
@@ -20899,10 +21145,10 @@
     </row>
     <row r="1101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1101" s="11" t="s">
-        <v>2263</v>
+        <v>2371</v>
       </c>
       <c r="D1101" s="8" t="s">
-        <v>2317</v>
+        <v>2441</v>
       </c>
       <c r="F1101" t="s">
         <v>3</v>
@@ -20910,10 +21156,10 @@
     </row>
     <row r="1102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1102" s="11" t="s">
-        <v>2264</v>
+        <v>2372</v>
       </c>
       <c r="D1102" s="8" t="s">
-        <v>2318</v>
+        <v>2441</v>
       </c>
       <c r="F1102" t="s">
         <v>3</v>
@@ -20921,10 +21167,10 @@
     </row>
     <row r="1103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1103" s="11" t="s">
-        <v>2265</v>
+        <v>2373</v>
       </c>
       <c r="D1103" s="8" t="s">
-        <v>2319</v>
+        <v>2441</v>
       </c>
       <c r="F1103" t="s">
         <v>3</v>
@@ -20932,10 +21178,10 @@
     </row>
     <row r="1104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1104" s="11" t="s">
-        <v>2266</v>
+        <v>2374</v>
       </c>
       <c r="D1104" s="8" t="s">
-        <v>2320</v>
+        <v>2441</v>
       </c>
       <c r="F1104" t="s">
         <v>3</v>
@@ -20943,10 +21189,10 @@
     </row>
     <row r="1105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1105" s="11" t="s">
-        <v>2267</v>
+        <v>2375</v>
       </c>
       <c r="D1105" s="8" t="s">
-        <v>2321</v>
+        <v>2441</v>
       </c>
       <c r="F1105" t="s">
         <v>3</v>
@@ -20954,10 +21200,10 @@
     </row>
     <row r="1106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1106" s="11" t="s">
-        <v>2268</v>
+        <v>2376</v>
       </c>
       <c r="D1106" s="8" t="s">
-        <v>2322</v>
+        <v>2441</v>
       </c>
       <c r="F1106" t="s">
         <v>3</v>
@@ -20965,10 +21211,10 @@
     </row>
     <row r="1107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1107" s="11" t="s">
-        <v>2269</v>
+        <v>2377</v>
       </c>
       <c r="D1107" s="8" t="s">
-        <v>2323</v>
+        <v>2441</v>
       </c>
       <c r="F1107" t="s">
         <v>3</v>
@@ -20976,10 +21222,10 @@
     </row>
     <row r="1108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1108" s="11" t="s">
-        <v>2270</v>
+        <v>2378</v>
       </c>
       <c r="D1108" s="8" t="s">
-        <v>2324</v>
+        <v>2441</v>
       </c>
       <c r="F1108" t="s">
         <v>3</v>
@@ -20987,10 +21233,10 @@
     </row>
     <row r="1109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1109" s="11" t="s">
-        <v>2271</v>
+        <v>2379</v>
       </c>
       <c r="D1109" s="8" t="s">
-        <v>2325</v>
+        <v>2441</v>
       </c>
       <c r="F1109" t="s">
         <v>3</v>
@@ -20998,10 +21244,10 @@
     </row>
     <row r="1110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1110" s="11" t="s">
-        <v>2272</v>
+        <v>2380</v>
       </c>
       <c r="D1110" s="8" t="s">
-        <v>2326</v>
+        <v>2441</v>
       </c>
       <c r="F1110" t="s">
         <v>3</v>
@@ -21009,10 +21255,10 @@
     </row>
     <row r="1111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1111" s="11" t="s">
-        <v>2273</v>
+        <v>2381</v>
       </c>
       <c r="D1111" s="8" t="s">
-        <v>2327</v>
+        <v>2441</v>
       </c>
       <c r="F1111" t="s">
         <v>3</v>
@@ -21020,10 +21266,10 @@
     </row>
     <row r="1112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1112" s="11" t="s">
-        <v>2274</v>
+        <v>2382</v>
       </c>
       <c r="D1112" s="8" t="s">
-        <v>2328</v>
+        <v>2441</v>
       </c>
       <c r="F1112" t="s">
         <v>3</v>
@@ -21031,10 +21277,10 @@
     </row>
     <row r="1113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1113" s="11" t="s">
-        <v>2275</v>
+        <v>2383</v>
       </c>
       <c r="D1113" s="8" t="s">
-        <v>2329</v>
+        <v>2441</v>
       </c>
       <c r="F1113" t="s">
         <v>3</v>
@@ -21042,10 +21288,10 @@
     </row>
     <row r="1114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1114" s="11" t="s">
-        <v>2276</v>
+        <v>2384</v>
       </c>
       <c r="D1114" s="8" t="s">
-        <v>2330</v>
+        <v>2441</v>
       </c>
       <c r="F1114" t="s">
         <v>3</v>
@@ -21053,10 +21299,10 @@
     </row>
     <row r="1115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1115" s="11" t="s">
-        <v>2277</v>
+        <v>2385</v>
       </c>
       <c r="D1115" s="8" t="s">
-        <v>2331</v>
+        <v>2441</v>
       </c>
       <c r="F1115" t="s">
         <v>3</v>
@@ -21064,10 +21310,10 @@
     </row>
     <row r="1116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1116" s="11" t="s">
-        <v>2278</v>
+        <v>2386</v>
       </c>
       <c r="D1116" s="8" t="s">
-        <v>2332</v>
+        <v>2441</v>
       </c>
       <c r="F1116" t="s">
         <v>3</v>
@@ -21075,497 +21321,472 @@
     </row>
     <row r="1117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1117" s="11" t="s">
-        <v>2279</v>
+        <v>2387</v>
       </c>
       <c r="D1117" s="8" t="s">
-        <v>2333</v>
+        <v>2441</v>
       </c>
       <c r="F1117" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1118" s="11" t="s">
-        <v>2280</v>
+        <v>2388</v>
       </c>
       <c r="D1118" s="8" t="s">
-        <v>2334</v>
+        <v>2441</v>
       </c>
       <c r="F1118" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1119" s="11" t="s">
-        <v>2281</v>
+        <v>2389</v>
       </c>
       <c r="D1119" s="8" t="s">
-        <v>2335</v>
+        <v>2441</v>
       </c>
       <c r="F1119" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1120" s="11" t="s">
-        <v>2282</v>
+        <v>2390</v>
       </c>
       <c r="D1120" s="8" t="s">
-        <v>2336</v>
+        <v>2441</v>
       </c>
       <c r="F1120" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1121" s="11" t="s">
-        <v>2283</v>
+        <v>2391</v>
       </c>
       <c r="D1121" s="8" t="s">
-        <v>2337</v>
+        <v>2441</v>
       </c>
       <c r="F1121" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1122" s="11" t="s">
-        <v>2284</v>
+        <v>2392</v>
       </c>
       <c r="D1122" s="8" t="s">
-        <v>2338</v>
+        <v>2441</v>
       </c>
       <c r="F1122" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1123" s="11" t="s">
-        <v>2285</v>
+        <v>2393</v>
       </c>
       <c r="D1123" s="8" t="s">
-        <v>2339</v>
+        <v>2441</v>
       </c>
       <c r="F1123" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1124" s="11" t="s">
-        <v>2286</v>
+        <v>2394</v>
       </c>
       <c r="D1124" s="8" t="s">
-        <v>2340</v>
+        <v>2441</v>
       </c>
       <c r="F1124" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1125" s="11" t="s">
-        <v>2287</v>
+        <v>2395</v>
       </c>
       <c r="D1125" s="8" t="s">
-        <v>2341</v>
+        <v>2441</v>
       </c>
       <c r="F1125" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1126" s="11" t="s">
-        <v>2288</v>
+        <v>2396</v>
       </c>
       <c r="D1126" s="8" t="s">
-        <v>2342</v>
+        <v>2441</v>
       </c>
       <c r="F1126" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1127" s="11" t="s">
-        <v>2289</v>
+        <v>2397</v>
       </c>
       <c r="D1127" s="8" t="s">
-        <v>2343</v>
+        <v>2441</v>
       </c>
       <c r="F1127" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1128" s="11" t="s">
-        <v>2290</v>
+        <v>2398</v>
       </c>
       <c r="D1128" s="8" t="s">
-        <v>2344</v>
+        <v>2441</v>
       </c>
       <c r="F1128" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1129" s="11" t="s">
-        <v>2291</v>
+        <v>2399</v>
       </c>
       <c r="D1129" s="8" t="s">
-        <v>2345</v>
+        <v>2441</v>
       </c>
       <c r="F1129" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1130" s="11" t="s">
-        <v>2292</v>
+        <v>2400</v>
       </c>
       <c r="D1130" s="8" t="s">
-        <v>2346</v>
+        <v>2441</v>
       </c>
       <c r="F1130" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1131" s="11" t="s">
-        <v>2293</v>
+        <v>2401</v>
       </c>
       <c r="D1131" s="8" t="s">
-        <v>2347</v>
+        <v>2441</v>
       </c>
       <c r="F1131" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1132" s="11" t="s">
-        <v>2294</v>
+        <v>2402</v>
       </c>
       <c r="D1132" s="8" t="s">
-        <v>2348</v>
+        <v>2441</v>
       </c>
       <c r="F1132" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1133" s="11" t="s">
-        <v>2295</v>
+        <v>2403</v>
       </c>
       <c r="D1133" s="8" t="s">
-        <v>2349</v>
+        <v>2441</v>
       </c>
       <c r="F1133" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1134" s="11" t="s">
-        <v>2296</v>
+        <v>2404</v>
       </c>
       <c r="D1134" s="8" t="s">
-        <v>2350</v>
+        <v>2441</v>
       </c>
       <c r="F1134" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1135" s="11" t="s">
-        <v>2297</v>
+        <v>2405</v>
       </c>
       <c r="D1135" s="8" t="s">
-        <v>2351</v>
+        <v>2441</v>
       </c>
       <c r="F1135" t="s">
-        <v>246</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1136" s="11" t="s">
-        <v>2298</v>
+        <v>2406</v>
       </c>
       <c r="D1136" s="8" t="s">
-        <v>2352</v>
+        <v>2441</v>
       </c>
       <c r="F1136" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1137" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1137" s="11" t="s">
-        <v>2299</v>
+        <v>2407</v>
       </c>
       <c r="D1137" s="8" t="s">
-        <v>2353</v>
+        <v>2441</v>
       </c>
       <c r="F1137" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1138" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1138" s="11" t="s">
-        <v>2300</v>
+        <v>2408</v>
       </c>
       <c r="D1138" s="8" t="s">
-        <v>2354</v>
+        <v>2441</v>
       </c>
       <c r="F1138" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1139" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1139" s="11" t="s">
-        <v>2301</v>
+        <v>2409</v>
       </c>
       <c r="D1139" s="8" t="s">
-        <v>2355</v>
+        <v>2441</v>
       </c>
       <c r="F1139" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1140" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1140" s="11" t="s">
-        <v>2302</v>
+        <v>2410</v>
       </c>
       <c r="D1140" s="8" t="s">
-        <v>2356</v>
+        <v>2441</v>
       </c>
       <c r="F1140" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1141" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1141" s="11" t="s">
-        <v>2303</v>
+        <v>2411</v>
       </c>
       <c r="D1141" s="8" t="s">
-        <v>2357</v>
+        <v>2441</v>
       </c>
       <c r="F1141" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1142" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1142" s="11" t="s">
-        <v>2304</v>
+        <v>2412</v>
       </c>
       <c r="D1142" s="8" t="s">
-        <v>2358</v>
+        <v>2441</v>
       </c>
       <c r="F1142" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1143" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1143" s="11" t="s">
-        <v>2305</v>
+        <v>2413</v>
       </c>
       <c r="D1143" s="8" t="s">
-        <v>2359</v>
+        <v>2441</v>
       </c>
       <c r="F1143" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="1144" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1144" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1144" s="10"/>
-      <c r="C1144" s="6"/>
-      <c r="D1144" s="6"/>
-      <c r="E1144" s="6"/>
-    </row>
-    <row r="1145" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1144" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1144" s="11" t="s">
+        <v>2414</v>
+      </c>
+      <c r="D1144" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1145" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1145" t="s">
-        <v>34</v>
+        <v>2415</v>
+      </c>
+      <c r="D1145" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1145" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="1146" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1146" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1146" t="s">
-        <v>36</v>
+        <v>2416</v>
+      </c>
+      <c r="D1146" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1146" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="1147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1147" s="11" t="s">
-        <v>2169</v>
-      </c>
-      <c r="D1147" t="s">
-        <v>2173</v>
-      </c>
-      <c r="E1147" t="s">
-        <v>2172</v>
+        <v>2417</v>
+      </c>
+      <c r="D1147" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1147" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="1148" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1148" s="11" t="s">
-        <v>2170</v>
-      </c>
-      <c r="D1148" t="s">
-        <v>2174</v>
-      </c>
-      <c r="E1148" t="s">
-        <v>2172</v>
+        <v>2418</v>
+      </c>
+      <c r="D1148" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1148" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="1149" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1149" s="11" t="s">
-        <v>2171</v>
-      </c>
-      <c r="D1149" t="s">
-        <v>2175</v>
-      </c>
-      <c r="E1149" t="s">
-        <v>2172</v>
+        <v>2419</v>
+      </c>
+      <c r="D1149" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1149" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="1150" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1150" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1150" t="s">
-        <v>38</v>
+        <v>2420</v>
+      </c>
+      <c r="D1150" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1150" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1151" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1151" s="11" t="s">
-        <v>2179</v>
-      </c>
-      <c r="D1151" t="s">
-        <v>2182</v>
-      </c>
-      <c r="E1151" t="s">
-        <v>2172</v>
+        <v>2421</v>
+      </c>
+      <c r="D1151" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1151" t="s">
-        <v>2188</v>
-      </c>
-    </row>
-    <row r="1152" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1152" s="11" t="s">
-        <v>2180</v>
-      </c>
-      <c r="D1152" t="s">
-        <v>2183</v>
-      </c>
-      <c r="E1152" t="s">
-        <v>2172</v>
+        <v>2422</v>
+      </c>
+      <c r="D1152" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1152" t="s">
-        <v>2188</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1153" s="11" t="s">
-        <v>2181</v>
-      </c>
-      <c r="D1153" t="s">
-        <v>2184</v>
-      </c>
-      <c r="E1153" t="s">
-        <v>2172</v>
+        <v>2423</v>
+      </c>
+      <c r="D1153" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1153" t="s">
-        <v>2188</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1154" s="11" t="s">
-        <v>2176</v>
-      </c>
-      <c r="D1154" t="s">
-        <v>2185</v>
-      </c>
-      <c r="E1154" t="s">
-        <v>2172</v>
+        <v>2424</v>
+      </c>
+      <c r="D1154" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1154" t="s">
-        <v>2189</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1155" s="11" t="s">
-        <v>2177</v>
-      </c>
-      <c r="D1155" t="s">
-        <v>2186</v>
-      </c>
-      <c r="E1155" t="s">
-        <v>2172</v>
+        <v>2425</v>
+      </c>
+      <c r="D1155" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1155" t="s">
-        <v>2189</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1156" s="11" t="s">
-        <v>2178</v>
-      </c>
-      <c r="D1156" t="s">
-        <v>2187</v>
-      </c>
-      <c r="E1156" t="s">
-        <v>2172</v>
+        <v>2426</v>
+      </c>
+      <c r="D1156" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1156" t="s">
-        <v>2189</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1157" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1157" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1157" t="s">
-        <v>30</v>
+        <v>2427</v>
+      </c>
+      <c r="D1157" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1157" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1158" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1158" t="s">
-        <v>42</v>
+        <v>2428</v>
+      </c>
+      <c r="D1158" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1158" t="s">
-        <v>2190</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1159" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1159" s="11" t="s">
-        <v>2191</v>
-      </c>
-      <c r="D1159" t="s">
-        <v>2194</v>
+        <v>2429</v>
+      </c>
+      <c r="D1159" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1159" t="s">
         <v>3</v>
@@ -21573,10 +21794,10 @@
     </row>
     <row r="1160" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1160" s="11" t="s">
-        <v>2192</v>
-      </c>
-      <c r="D1160" t="s">
-        <v>2195</v>
+        <v>2430</v>
+      </c>
+      <c r="D1160" s="8" t="s">
+        <v>2441</v>
       </c>
       <c r="F1160" t="s">
         <v>3</v>
@@ -21584,12 +21805,928 @@
     </row>
     <row r="1161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1161" s="11" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D1161" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1161" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1162" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1162" s="11" t="s">
+        <v>2432</v>
+      </c>
+      <c r="D1162" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1162" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1163" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1163" s="11" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D1163" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1163" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1164" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1164" s="11" t="s">
+        <v>2434</v>
+      </c>
+      <c r="D1164" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1164" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1165" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1165" s="11" t="s">
+        <v>2435</v>
+      </c>
+      <c r="D1165" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1165" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1166" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1166" s="11" t="s">
+        <v>2436</v>
+      </c>
+      <c r="D1166" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1166" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1167" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1167" s="11" t="s">
+        <v>2437</v>
+      </c>
+      <c r="D1167" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1167" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1168" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1168" s="11" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D1168" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1168" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1169" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1169" s="11" t="s">
+        <v>2439</v>
+      </c>
+      <c r="D1169" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1169" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1170" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1170" s="11" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D1170" s="8" t="s">
+        <v>2441</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1171" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1171" s="11" t="s">
+        <v>2252</v>
+      </c>
+      <c r="D1171" s="8" t="s">
+        <v>2306</v>
+      </c>
+      <c r="F1171" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1172" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1172" s="11" t="s">
+        <v>2253</v>
+      </c>
+      <c r="D1172" s="8" t="s">
+        <v>2307</v>
+      </c>
+      <c r="F1172" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1173" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1173" s="11" t="s">
+        <v>2254</v>
+      </c>
+      <c r="D1173" s="8" t="s">
+        <v>2308</v>
+      </c>
+      <c r="F1173" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1174" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1174" s="11" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D1174" s="8" t="s">
+        <v>2309</v>
+      </c>
+      <c r="F1174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1175" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1175" s="11" t="s">
+        <v>2256</v>
+      </c>
+      <c r="D1175" s="8" t="s">
+        <v>2310</v>
+      </c>
+      <c r="F1175" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1176" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1176" s="11" t="s">
+        <v>2257</v>
+      </c>
+      <c r="D1176" s="8" t="s">
+        <v>2311</v>
+      </c>
+      <c r="F1176" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1177" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1177" s="11" t="s">
+        <v>2258</v>
+      </c>
+      <c r="D1177" s="8" t="s">
+        <v>2312</v>
+      </c>
+      <c r="F1177" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1178" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1178" s="11" t="s">
+        <v>2259</v>
+      </c>
+      <c r="D1178" s="8" t="s">
+        <v>2313</v>
+      </c>
+      <c r="F1178" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1179" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1179" s="11" t="s">
+        <v>2260</v>
+      </c>
+      <c r="D1179" s="8" t="s">
+        <v>2314</v>
+      </c>
+      <c r="F1179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1180" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1180" s="11" t="s">
+        <v>2261</v>
+      </c>
+      <c r="D1180" s="8" t="s">
+        <v>2315</v>
+      </c>
+      <c r="F1180" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1181" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1181" s="11" t="s">
+        <v>2262</v>
+      </c>
+      <c r="D1181" s="8" t="s">
+        <v>2316</v>
+      </c>
+      <c r="F1181" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1182" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1182" s="11" t="s">
+        <v>2263</v>
+      </c>
+      <c r="D1182" s="8" t="s">
+        <v>2317</v>
+      </c>
+      <c r="F1182" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1183" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1183" s="11" t="s">
+        <v>2264</v>
+      </c>
+      <c r="D1183" s="8" t="s">
+        <v>2318</v>
+      </c>
+      <c r="F1183" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1184" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1184" s="11" t="s">
+        <v>2265</v>
+      </c>
+      <c r="D1184" s="8" t="s">
+        <v>2319</v>
+      </c>
+      <c r="F1184" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1185" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1185" s="11" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D1185" s="8" t="s">
+        <v>2320</v>
+      </c>
+      <c r="F1185" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1186" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1186" s="11" t="s">
+        <v>2267</v>
+      </c>
+      <c r="D1186" s="8" t="s">
+        <v>2321</v>
+      </c>
+      <c r="F1186" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1187" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1187" s="11" t="s">
+        <v>2268</v>
+      </c>
+      <c r="D1187" s="8" t="s">
+        <v>2322</v>
+      </c>
+      <c r="F1187" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1188" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1188" s="11" t="s">
+        <v>2269</v>
+      </c>
+      <c r="D1188" s="8" t="s">
+        <v>2323</v>
+      </c>
+      <c r="F1188" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1189" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1189" s="11" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D1189" s="8" t="s">
+        <v>2324</v>
+      </c>
+      <c r="F1189" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1190" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1190" s="11" t="s">
+        <v>2271</v>
+      </c>
+      <c r="D1190" s="8" t="s">
+        <v>2325</v>
+      </c>
+      <c r="F1190" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1191" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1191" s="11" t="s">
+        <v>2272</v>
+      </c>
+      <c r="D1191" s="8" t="s">
+        <v>2326</v>
+      </c>
+      <c r="F1191" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1192" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1192" s="11" t="s">
+        <v>2273</v>
+      </c>
+      <c r="D1192" s="8" t="s">
+        <v>2327</v>
+      </c>
+      <c r="F1192" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1193" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1193" s="11" t="s">
+        <v>2274</v>
+      </c>
+      <c r="D1193" s="8" t="s">
+        <v>2328</v>
+      </c>
+      <c r="F1193" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1194" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1194" s="11" t="s">
+        <v>2275</v>
+      </c>
+      <c r="D1194" s="8" t="s">
+        <v>2329</v>
+      </c>
+      <c r="F1194" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1195" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1195" s="11" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D1195" s="8" t="s">
+        <v>2330</v>
+      </c>
+      <c r="F1195" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1196" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1196" s="11" t="s">
+        <v>2277</v>
+      </c>
+      <c r="D1196" s="8" t="s">
+        <v>2331</v>
+      </c>
+      <c r="F1196" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1197" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1197" s="11" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D1197" s="8" t="s">
+        <v>2332</v>
+      </c>
+      <c r="F1197" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1198" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1198" s="11" t="s">
+        <v>2279</v>
+      </c>
+      <c r="D1198" s="8" t="s">
+        <v>2333</v>
+      </c>
+      <c r="F1198" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1199" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1199" s="11" t="s">
+        <v>2280</v>
+      </c>
+      <c r="D1199" s="8" t="s">
+        <v>2334</v>
+      </c>
+      <c r="F1199" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1200" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1200" s="11" t="s">
+        <v>2281</v>
+      </c>
+      <c r="D1200" s="8" t="s">
+        <v>2335</v>
+      </c>
+      <c r="F1200" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1201" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1201" s="11" t="s">
+        <v>2282</v>
+      </c>
+      <c r="D1201" s="8" t="s">
+        <v>2336</v>
+      </c>
+      <c r="F1201" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1202" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1202" s="11" t="s">
+        <v>2283</v>
+      </c>
+      <c r="D1202" s="8" t="s">
+        <v>2337</v>
+      </c>
+      <c r="F1202" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1203" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1203" s="11" t="s">
+        <v>2284</v>
+      </c>
+      <c r="D1203" s="8" t="s">
+        <v>2338</v>
+      </c>
+      <c r="F1203" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1204" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1204" s="11" t="s">
+        <v>2285</v>
+      </c>
+      <c r="D1204" s="8" t="s">
+        <v>2339</v>
+      </c>
+      <c r="F1204" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1205" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1205" s="11" t="s">
+        <v>2286</v>
+      </c>
+      <c r="D1205" s="8" t="s">
+        <v>2340</v>
+      </c>
+      <c r="F1205" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1206" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1206" s="11" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D1206" s="8" t="s">
+        <v>2341</v>
+      </c>
+      <c r="F1206" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1207" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1207" s="11" t="s">
+        <v>2288</v>
+      </c>
+      <c r="D1207" s="8" t="s">
+        <v>2342</v>
+      </c>
+      <c r="F1207" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1208" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1208" s="11" t="s">
+        <v>2289</v>
+      </c>
+      <c r="D1208" s="8" t="s">
+        <v>2343</v>
+      </c>
+      <c r="F1208" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1209" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1209" s="11" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D1209" s="8" t="s">
+        <v>2344</v>
+      </c>
+      <c r="F1209" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1210" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1210" s="11" t="s">
+        <v>2291</v>
+      </c>
+      <c r="D1210" s="8" t="s">
+        <v>2345</v>
+      </c>
+      <c r="F1210" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1211" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1211" s="11" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D1211" s="8" t="s">
+        <v>2346</v>
+      </c>
+      <c r="F1211" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1212" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1212" s="11" t="s">
+        <v>2293</v>
+      </c>
+      <c r="D1212" s="8" t="s">
+        <v>2347</v>
+      </c>
+      <c r="F1212" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1213" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1213" s="11" t="s">
+        <v>2294</v>
+      </c>
+      <c r="D1213" s="8" t="s">
+        <v>2348</v>
+      </c>
+      <c r="F1213" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1214" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1214" s="11" t="s">
+        <v>2295</v>
+      </c>
+      <c r="D1214" s="8" t="s">
+        <v>2349</v>
+      </c>
+      <c r="F1214" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1215" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1215" s="11" t="s">
+        <v>2296</v>
+      </c>
+      <c r="D1215" s="8" t="s">
+        <v>2350</v>
+      </c>
+      <c r="F1215" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1216" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1216" s="11" t="s">
+        <v>2297</v>
+      </c>
+      <c r="D1216" s="8" t="s">
+        <v>2351</v>
+      </c>
+      <c r="F1216" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1217" s="11" t="s">
+        <v>2298</v>
+      </c>
+      <c r="D1217" s="8" t="s">
+        <v>2352</v>
+      </c>
+      <c r="F1217" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1218" s="11" t="s">
+        <v>2299</v>
+      </c>
+      <c r="D1218" s="8" t="s">
+        <v>2353</v>
+      </c>
+      <c r="F1218" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1219" s="11" t="s">
+        <v>2300</v>
+      </c>
+      <c r="D1219" s="8" t="s">
+        <v>2354</v>
+      </c>
+      <c r="F1219" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1220" s="11" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D1220" s="8" t="s">
+        <v>2355</v>
+      </c>
+      <c r="F1220" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1221" s="11" t="s">
+        <v>2302</v>
+      </c>
+      <c r="D1221" s="8" t="s">
+        <v>2356</v>
+      </c>
+      <c r="F1221" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1222" s="11" t="s">
+        <v>2303</v>
+      </c>
+      <c r="D1222" s="8" t="s">
+        <v>2357</v>
+      </c>
+      <c r="F1222" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1223" s="11" t="s">
+        <v>2304</v>
+      </c>
+      <c r="D1223" s="8" t="s">
+        <v>2358</v>
+      </c>
+      <c r="F1223" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1224" s="11" t="s">
+        <v>2305</v>
+      </c>
+      <c r="D1224" s="8" t="s">
+        <v>2359</v>
+      </c>
+      <c r="F1224" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1225" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1225" s="10"/>
+      <c r="C1225" s="6"/>
+      <c r="D1225" s="6"/>
+      <c r="E1225" s="6"/>
+    </row>
+    <row r="1226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1226" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1226" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1227" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1227" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1227" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1228" s="11" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D1228" t="s">
+        <v>2173</v>
+      </c>
+      <c r="E1228" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1228" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1229" s="11" t="s">
+        <v>2170</v>
+      </c>
+      <c r="D1229" t="s">
+        <v>2174</v>
+      </c>
+      <c r="E1229" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1229" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1230" s="11" t="s">
+        <v>2171</v>
+      </c>
+      <c r="D1230" t="s">
+        <v>2175</v>
+      </c>
+      <c r="E1230" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1230" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1231" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1231" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1231" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1232" s="11" t="s">
+        <v>2179</v>
+      </c>
+      <c r="D1232" t="s">
+        <v>2182</v>
+      </c>
+      <c r="E1232" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1232" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="1233" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1233" s="11" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D1233" t="s">
+        <v>2183</v>
+      </c>
+      <c r="E1233" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1233" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="1234" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1234" s="11" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D1234" t="s">
+        <v>2184</v>
+      </c>
+      <c r="E1234" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1234" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="1235" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1235" s="11" t="s">
+        <v>2176</v>
+      </c>
+      <c r="D1235" t="s">
+        <v>2185</v>
+      </c>
+      <c r="E1235" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1235" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="1236" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1236" s="11" t="s">
+        <v>2177</v>
+      </c>
+      <c r="D1236" t="s">
+        <v>2186</v>
+      </c>
+      <c r="E1236" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1236" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="1237" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1237" s="11" t="s">
+        <v>2178</v>
+      </c>
+      <c r="D1237" t="s">
+        <v>2187</v>
+      </c>
+      <c r="E1237" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1237" t="s">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="1238" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1238" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1238" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1238" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1239" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1239" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1239" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1239" t="s">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="1240" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1240" s="11" t="s">
+        <v>2191</v>
+      </c>
+      <c r="D1240" t="s">
+        <v>2194</v>
+      </c>
+      <c r="F1240" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1241" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1241" s="11" t="s">
+        <v>2192</v>
+      </c>
+      <c r="D1241" t="s">
+        <v>2195</v>
+      </c>
+      <c r="F1241" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1242" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1242" s="11" t="s">
         <v>2193</v>
       </c>
-      <c r="D1161" t="s">
+      <c r="D1242" t="s">
         <v>2196</v>
       </c>
-      <c r="F1161" t="s">
+      <c r="F1242" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>